<commit_message>
Novas features para usuários
Features novas para evitar erros do usuário
</commit_message>
<xml_diff>
--- a/Backup.xlsx
+++ b/Backup.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C1:C1048576"/>
@@ -682,6 +682,59 @@
         <v/>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>26/06/2023 10:34</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="6">
+        <f>D6 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E6" s="6">
+        <f>B6 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="G6" s="6">
+        <f>F6 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I6" s="6">
+        <f>H6 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="K6" s="6">
+        <f>J6 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M6" s="6">
+        <f>L6 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="N6" s="6">
+        <f>C6+E6+G6+I6+K6+M6</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D1:E1"/>

</xml_diff>

<commit_message>
Melhorias na leitura de dados
</commit_message>
<xml_diff>
--- a/Backup.xlsx
+++ b/Backup.xlsx
@@ -581,20 +581,57 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n"/>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="9" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="9" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="9" t="n"/>
-      <c r="J3" s="3" t="n"/>
-      <c r="K3" s="9" t="n"/>
-      <c r="L3" s="3" t="n"/>
-      <c r="M3" s="9" t="n"/>
-      <c r="N3" s="9" t="n"/>
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>10/07/2023 15:31</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C3" s="9">
+        <f>B3 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="9">
+        <f>D3 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G3" s="9">
+        <f>F3 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I3" s="9">
+        <f>H3 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K3" s="9">
+        <f>J3 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="M3" s="9">
+        <f>L3 * 600 / 100 *100</f>
+        <v/>
+      </c>
+      <c r="N3" s="9">
+        <f>C3+E3+G3+I3+K3+M3</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>

</xml_diff>